<commit_message>
Weitere Bilder ausgemessen um die Excel fertig zu machen
</commit_message>
<xml_diff>
--- a/Bildervorbearbeitung/Bilder/xlsx/Porositaet_P_006_quad.xlsx
+++ b/Bildervorbearbeitung/Bilder/xlsx/Porositaet_P_006_quad.xlsx
@@ -448,1821 +448,1821 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_1.png</t>
+          <t>P_006_quad_crp_x1_y1.png</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.09039999999999999</v>
+        <v>0.1236</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_2.png</t>
+          <t>P_006_quad_crp_x1_y2.png</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0804</v>
+        <v>0.1048</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_3.png</t>
+          <t>P_006_quad_crp_x1_y3.png</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0216</v>
+        <v>0.0344</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_4.png</t>
+          <t>P_006_quad_crp_x1_y4.png</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.15</v>
+        <v>0.1728</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_5.png</t>
+          <t>P_006_quad_crp_x1_y5.png</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1436</v>
+        <v>0.1852</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_6.png</t>
+          <t>P_006_quad_crp_x1_y6.png</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.11</v>
+        <v>0.1516</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_7.png</t>
+          <t>P_006_quad_crp_x1_y7.png</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0256</v>
+        <v>0.0396</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_8.png</t>
+          <t>P_006_quad_crp_x1_y8.png</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0532</v>
+        <v>0.0824</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_9.png</t>
+          <t>P_006_quad_crp_x1_y9.png</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.1172</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_10.png</t>
+          <t>P_006_quad_crp_x1_y10.png</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.04960000000000001</v>
+        <v>0.06520000000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_11.png</t>
+          <t>P_006_quad_crp_x1_y11.png</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.052</v>
+        <v>0.1048</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_12.png</t>
+          <t>P_006_quad_crp_x1_y12.png</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.326</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_13.png</t>
+          <t>P_006_quad_crp_x1_y13.png</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0588</v>
+        <v>0.09279999999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_1_y_14.png</t>
+          <t>P_006_quad_crp_x1_y14.png</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0212</v>
+        <v>0.034</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_1.png</t>
+          <t>P_006_quad_crp_x2_y1.png</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1976</v>
+        <v>0.236</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_2.png</t>
+          <t>P_006_quad_crp_x2_y2.png</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.0484</v>
+        <v>0.07479999999999999</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_3.png</t>
+          <t>P_006_quad_crp_x2_y3.png</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1124</v>
+        <v>0.1596</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_4.png</t>
+          <t>P_006_quad_crp_x2_y4.png</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.152</v>
+        <v>0.1824</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_5.png</t>
+          <t>P_006_quad_crp_x2_y5.png</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1892</v>
+        <v>0.2628</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_6.png</t>
+          <t>P_006_quad_crp_x2_y6.png</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.0132</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_7.png</t>
+          <t>P_006_quad_crp_x2_y7.png</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.2128</v>
+        <v>0.2512</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_8.png</t>
+          <t>P_006_quad_crp_x2_y8.png</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.0672</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_9.png</t>
+          <t>P_006_quad_crp_x2_y9.png</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.06319999999999999</v>
+        <v>0.1008</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_10.png</t>
+          <t>P_006_quad_crp_x2_y10.png</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1264</v>
+        <v>0.1576</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_11.png</t>
+          <t>P_006_quad_crp_x2_y11.png</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.0328</v>
+        <v>0.06560000000000001</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_12.png</t>
+          <t>P_006_quad_crp_x2_y12.png</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.2528</v>
+        <v>0.3128</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_13.png</t>
+          <t>P_006_quad_crp_x2_y13.png</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.1692</v>
+        <v>0.2016</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_2_y_14.png</t>
+          <t>P_006_quad_crp_x2_y14.png</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.022</v>
+        <v>0.0448</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_1.png</t>
+          <t>P_006_quad_crp_x3_y1.png</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.0212</v>
+        <v>0.0464</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_2.png</t>
+          <t>P_006_quad_crp_x3_y2.png</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.01</v>
+        <v>0.0332</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_3.png</t>
+          <t>P_006_quad_crp_x3_y3.png</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.008399999999999999</v>
+        <v>0.0248</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_4.png</t>
+          <t>P_006_quad_crp_x3_y4.png</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1516</v>
+        <v>0.1808</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_5.png</t>
+          <t>P_006_quad_crp_x3_y5.png</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1404</v>
+        <v>0.1888</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_6.png</t>
+          <t>P_006_quad_crp_x3_y6.png</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.0412</v>
+        <v>0.0588</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_7.png</t>
+          <t>P_006_quad_crp_x3_y7.png</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.198</v>
+        <v>0.2284</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_8.png</t>
+          <t>P_006_quad_crp_x3_y8.png</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.1652</v>
+        <v>0.2052</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_9.png</t>
+          <t>P_006_quad_crp_x3_y9.png</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.1932</v>
+        <v>0.3024</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_10.png</t>
+          <t>P_006_quad_crp_x3_y10.png</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.0252</v>
+        <v>0.0444</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_11.png</t>
+          <t>P_006_quad_crp_x3_y11.png</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.106</v>
+        <v>0.1624</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_12.png</t>
+          <t>P_006_quad_crp_x3_y12.png</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.1276</v>
+        <v>0.1892</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_13.png</t>
+          <t>P_006_quad_crp_x3_y13.png</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.0588</v>
+        <v>0.08639999999999999</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_3_y_14.png</t>
+          <t>P_006_quad_crp_x3_y14.png</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.0136</v>
+        <v>0.0292</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_1.png</t>
+          <t>P_006_quad_crp_x4_y1.png</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.2084</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_2.png</t>
+          <t>P_006_quad_crp_x4_y2.png</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.0224</v>
+        <v>0.0404</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_3.png</t>
+          <t>P_006_quad_crp_x4_y3.png</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.0152</v>
+        <v>0.0264</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_4.png</t>
+          <t>P_006_quad_crp_x4_y4.png</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.0192</v>
+        <v>0.0296</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_5.png</t>
+          <t>P_006_quad_crp_x4_y5.png</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.06279999999999999</v>
+        <v>0.0832</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_6.png</t>
+          <t>P_006_quad_crp_x4_y6.png</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.0832</v>
+        <v>0.1036</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_7.png</t>
+          <t>P_006_quad_crp_x4_y7.png</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.0336</v>
+        <v>0.0456</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_8.png</t>
+          <t>P_006_quad_crp_x4_y8.png</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.008399999999999999</v>
+        <v>0.0168</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_9.png</t>
+          <t>P_006_quad_crp_x4_y9.png</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.0956</v>
+        <v>0.1324</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_10.png</t>
+          <t>P_006_quad_crp_x4_y10.png</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.256</v>
+        <v>0.2896</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_11.png</t>
+          <t>P_006_quad_crp_x4_y11.png</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.0344</v>
+        <v>0.0592</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_12.png</t>
+          <t>P_006_quad_crp_x4_y12.png</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.02</v>
+        <v>0.05159999999999999</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_13.png</t>
+          <t>P_006_quad_crp_x4_y13.png</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.0488</v>
+        <v>0.0712</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_4_y_14.png</t>
+          <t>P_006_quad_crp_x4_y14.png</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.1356</v>
+        <v>0.1688</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_1.png</t>
+          <t>P_006_quad_crp_x5_y1.png</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.04</v>
+        <v>0.05959999999999999</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_2.png</t>
+          <t>P_006_quad_crp_x5_y2.png</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.0372</v>
+        <v>0.0504</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_3.png</t>
+          <t>P_006_quad_crp_x5_y3.png</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0304</v>
+        <v>0.0508</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_4.png</t>
+          <t>P_006_quad_crp_x5_y4.png</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.0112</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_5.png</t>
+          <t>P_006_quad_crp_x5_y5.png</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.0492</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_6.png</t>
+          <t>P_006_quad_crp_x5_y6.png</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.07919999999999999</v>
+        <v>0.1092</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_7.png</t>
+          <t>P_006_quad_crp_x5_y7.png</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.0316</v>
+        <v>0.0492</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_8.png</t>
+          <t>P_006_quad_crp_x5_y8.png</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.0548</v>
+        <v>0.0824</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_9.png</t>
+          <t>P_006_quad_crp_x5_y9.png</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.0572</v>
+        <v>0.07240000000000001</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_10.png</t>
+          <t>P_006_quad_crp_x5_y10.png</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.1068</v>
+        <v>0.1316</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_11.png</t>
+          <t>P_006_quad_crp_x5_y11.png</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.7396</v>
+        <v>0.8736</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_12.png</t>
+          <t>P_006_quad_crp_x5_y12.png</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.0196</v>
+        <v>0.0408</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_13.png</t>
+          <t>P_006_quad_crp_x5_y13.png</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.1216</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_5_y_14.png</t>
+          <t>P_006_quad_crp_x5_y14.png</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.0144</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_1.png</t>
+          <t>P_006_quad_crp_x6_y1.png</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.0616</v>
+        <v>0.08760000000000001</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_2.png</t>
+          <t>P_006_quad_crp_x6_y2.png</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.06999999999999999</v>
+        <v>0.0956</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_3.png</t>
+          <t>P_006_quad_crp_x6_y3.png</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.0832</v>
+        <v>0.09719999999999999</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_4.png</t>
+          <t>P_006_quad_crp_x6_y4.png</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.0092</v>
+        <v>0.0212</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_5.png</t>
+          <t>P_006_quad_crp_x6_y5.png</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.0068</v>
+        <v>0.0148</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_6.png</t>
+          <t>P_006_quad_crp_x6_y6.png</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.04960000000000001</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_7.png</t>
+          <t>P_006_quad_crp_x6_y7.png</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.0316</v>
+        <v>0.0484</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_8.png</t>
+          <t>P_006_quad_crp_x6_y8.png</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.9608</v>
+        <v>1.0172</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_9.png</t>
+          <t>P_006_quad_crp_x6_y9.png</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.0412</v>
+        <v>0.06759999999999999</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_10.png</t>
+          <t>P_006_quad_crp_x6_y10.png</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.1332</v>
+        <v>0.1744</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_11.png</t>
+          <t>P_006_quad_crp_x6_y11.png</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.1536</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_12.png</t>
+          <t>P_006_quad_crp_x6_y12.png</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.0716</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_13.png</t>
+          <t>P_006_quad_crp_x6_y13.png</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.0512</v>
+        <v>0.0648</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_6_y_14.png</t>
+          <t>P_006_quad_crp_x6_y14.png</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.0308</v>
+        <v>0.0552</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_1.png</t>
+          <t>P_006_quad_crp_x7_y1.png</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.0668</v>
+        <v>0.0912</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_2.png</t>
+          <t>P_006_quad_crp_x7_y2.png</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.194</v>
+        <v>0.228</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_3.png</t>
+          <t>P_006_quad_crp_x7_y3.png</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.112</v>
+        <v>0.146</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_4.png</t>
+          <t>P_006_quad_crp_x7_y4.png</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.0196</v>
+        <v>0.0392</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_5.png</t>
+          <t>P_006_quad_crp_x7_y5.png</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.022</v>
+        <v>0.03759999999999999</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_6.png</t>
+          <t>P_006_quad_crp_x7_y6.png</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.08639999999999999</v>
+        <v>0.1112</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_7.png</t>
+          <t>P_006_quad_crp_x7_y7.png</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.2164</v>
+        <v>0.266</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_8.png</t>
+          <t>P_006_quad_crp_x7_y8.png</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.0052</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_9.png</t>
+          <t>P_006_quad_crp_x7_y9.png</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.0616</v>
+        <v>0.0956</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_10.png</t>
+          <t>P_006_quad_crp_x7_y10.png</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.136</v>
+        <v>0.1776</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_11.png</t>
+          <t>P_006_quad_crp_x7_y11.png</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.2552</v>
+        <v>0.2856</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_12.png</t>
+          <t>P_006_quad_crp_x7_y12.png</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.03759999999999999</v>
+        <v>0.06080000000000001</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_13.png</t>
+          <t>P_006_quad_crp_x7_y13.png</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.0092</v>
+        <v>0.0232</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_7_y_14.png</t>
+          <t>P_006_quad_crp_x7_y14.png</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.0148</v>
+        <v>0.0444</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_1.png</t>
+          <t>P_006_quad_crp_x8_y1.png</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.1188</v>
+        <v>0.1468</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_2.png</t>
+          <t>P_006_quad_crp_x8_y2.png</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.0612</v>
+        <v>0.08639999999999999</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_3.png</t>
+          <t>P_006_quad_crp_x8_y3.png</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.0144</v>
+        <v>0.0296</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_4.png</t>
+          <t>P_006_quad_crp_x8_y4.png</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.008</v>
+        <v>0.0176</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_5.png</t>
+          <t>P_006_quad_crp_x8_y5.png</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.1532</v>
+        <v>0.1792</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_6.png</t>
+          <t>P_006_quad_crp_x8_y6.png</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.2632</v>
+        <v>0.2928</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_7.png</t>
+          <t>P_006_quad_crp_x8_y7.png</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.0164</v>
+        <v>0.0296</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_8.png</t>
+          <t>P_006_quad_crp_x8_y8.png</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.0428</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_9.png</t>
+          <t>P_006_quad_crp_x8_y9.png</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.1444</v>
+        <v>0.1864</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_10.png</t>
+          <t>P_006_quad_crp_x8_y10.png</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.1652</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_11.png</t>
+          <t>P_006_quad_crp_x8_y11.png</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.0716</v>
+        <v>0.1124</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_12.png</t>
+          <t>P_006_quad_crp_x8_y12.png</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.1032</v>
+        <v>0.1328</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_13.png</t>
+          <t>P_006_quad_crp_x8_y13.png</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.2948</v>
+        <v>0.3588</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_8_y_14.png</t>
+          <t>P_006_quad_crp_x8_y14.png</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.1232</v>
+        <v>0.1632</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_1.png</t>
+          <t>P_006_quad_crp_x9_y1.png</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.008</v>
+        <v>0.0188</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_2.png</t>
+          <t>P_006_quad_crp_x9_y2.png</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.004</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_3.png</t>
+          <t>P_006_quad_crp_x9_y3.png</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.0172</v>
+        <v>0.0304</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_4.png</t>
+          <t>P_006_quad_crp_x9_y4.png</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.0448</v>
+        <v>0.0704</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_5.png</t>
+          <t>P_006_quad_crp_x9_y5.png</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.1528</v>
+        <v>0.1832</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_6.png</t>
+          <t>P_006_quad_crp_x9_y6.png</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.052</v>
+        <v>0.06999999999999999</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_7.png</t>
+          <t>P_006_quad_crp_x9_y7.png</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.1012</v>
+        <v>0.1184</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_8.png</t>
+          <t>P_006_quad_crp_x9_y8.png</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.0372</v>
+        <v>0.0552</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_9.png</t>
+          <t>P_006_quad_crp_x9_y9.png</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.1324</v>
+        <v>0.1692</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_10.png</t>
+          <t>P_006_quad_crp_x9_y10.png</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.2296</v>
+        <v>0.2636</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_11.png</t>
+          <t>P_006_quad_crp_x9_y11.png</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.3144</v>
+        <v>0.4072</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_12.png</t>
+          <t>P_006_quad_crp_x9_y12.png</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.048</v>
+        <v>0.0716</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_13.png</t>
+          <t>P_006_quad_crp_x9_y13.png</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>0.1396</v>
+        <v>0.1728</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_9_y_14.png</t>
+          <t>P_006_quad_crp_x9_y14.png</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.1024</v>
+        <v>0.1332</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_1.png</t>
+          <t>P_006_quad_crp_x10_y1.png</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>0.0104</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_2.png</t>
+          <t>P_006_quad_crp_x10_y2.png</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.0148</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_3.png</t>
+          <t>P_006_quad_crp_x10_y3.png</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.0872</v>
+        <v>0.1156</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_4.png</t>
+          <t>P_006_quad_crp_x10_y4.png</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.006399999999999999</v>
+        <v>0.0164</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_5.png</t>
+          <t>P_006_quad_crp_x10_y5.png</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_6.png</t>
+          <t>P_006_quad_crp_x10_y6.png</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.0616</v>
+        <v>0.0776</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_7.png</t>
+          <t>P_006_quad_crp_x10_y7.png</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.0772</v>
+        <v>0.0944</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_8.png</t>
+          <t>P_006_quad_crp_x10_y8.png</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.0696</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_9.png</t>
+          <t>P_006_quad_crp_x10_y9.png</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.0224</v>
+        <v>0.0448</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_10.png</t>
+          <t>P_006_quad_crp_x10_y10.png</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.098</v>
+        <v>0.1312</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_11.png</t>
+          <t>P_006_quad_crp_x10_y11.png</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.0204</v>
+        <v>0.0456</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_12.png</t>
+          <t>P_006_quad_crp_x10_y12.png</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.0776</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_13.png</t>
+          <t>P_006_quad_crp_x10_y13.png</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.1104</v>
+        <v>0.1612</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_10_y_14.png</t>
+          <t>P_006_quad_crp_x10_y14.png</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.1896</v>
+        <v>0.2636</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_1.png</t>
+          <t>P_006_quad_crp_x11_y1.png</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.0504</v>
+        <v>0.0872</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_2.png</t>
+          <t>P_006_quad_crp_x11_y2.png</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.0108</v>
+        <v>0.0216</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_3.png</t>
+          <t>P_006_quad_crp_x11_y3.png</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.1328</v>
+        <v>0.1752</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_4.png</t>
+          <t>P_006_quad_crp_x11_y4.png</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.0384</v>
+        <v>0.0648</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_5.png</t>
+          <t>P_006_quad_crp_x11_y5.png</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.0868</v>
+        <v>0.1096</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_6.png</t>
+          <t>P_006_quad_crp_x11_y6.png</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.0092</v>
+        <v>0.0256</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_7.png</t>
+          <t>P_006_quad_crp_x11_y7.png</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.0052</v>
+        <v>0.0152</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_8.png</t>
+          <t>P_006_quad_crp_x11_y8.png</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.0256</v>
+        <v>0.0384</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_9.png</t>
+          <t>P_006_quad_crp_x11_y9.png</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.0176</v>
+        <v>0.0464</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_10.png</t>
+          <t>P_006_quad_crp_x11_y10.png</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.07479999999999999</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_11.png</t>
+          <t>P_006_quad_crp_x11_y11.png</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.0664</v>
+        <v>0.0916</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_12.png</t>
+          <t>P_006_quad_crp_x11_y12.png</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>0.5232</v>
+        <v>0.5868</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_13.png</t>
+          <t>P_006_quad_crp_x11_y13.png</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.182</v>
+        <v>0.208</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_11_y_14.png</t>
+          <t>P_006_quad_crp_x11_y14.png</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0.0232</v>
+        <v>0.04960000000000001</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_1.png</t>
+          <t>P_006_quad_crp_x12_y1.png</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.022</v>
+        <v>0.0556</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_2.png</t>
+          <t>P_006_quad_crp_x12_y2.png</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.0848</v>
+        <v>0.118</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_3.png</t>
+          <t>P_006_quad_crp_x12_y3.png</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.124</v>
+        <v>0.1584</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_4.png</t>
+          <t>P_006_quad_crp_x12_y4.png</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.1812</v>
+        <v>0.2072</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_5.png</t>
+          <t>P_006_quad_crp_x12_y5.png</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.08800000000000001</v>
+        <v>0.1104</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_6.png</t>
+          <t>P_006_quad_crp_x12_y6.png</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.0152</v>
+        <v>0.0292</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_7.png</t>
+          <t>P_006_quad_crp_x12_y7.png</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.0348</v>
+        <v>0.0544</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_8.png</t>
+          <t>P_006_quad_crp_x12_y8.png</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.0268</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_9.png</t>
+          <t>P_006_quad_crp_x12_y9.png</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.1228</v>
+        <v>0.1652</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_10.png</t>
+          <t>P_006_quad_crp_x12_y10.png</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.0692</v>
+        <v>0.1008</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_11.png</t>
+          <t>P_006_quad_crp_x12_y11.png</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.0544</v>
+        <v>0.0832</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_12.png</t>
+          <t>P_006_quad_crp_x12_y12.png</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.02</v>
+        <v>0.0452</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_13.png</t>
+          <t>P_006_quad_crp_x12_y13.png</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.2264</v>
+        <v>0.296</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_12_y_14.png</t>
+          <t>P_006_quad_crp_x12_y14.png</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.0196</v>
+        <v>0.0388</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_1.png</t>
+          <t>P_006_quad_crp_x13_y1.png</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.1188</v>
+        <v>0.1692</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_2.png</t>
+          <t>P_006_quad_crp_x13_y2.png</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.0216</v>
+        <v>0.0624</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_3.png</t>
+          <t>P_006_quad_crp_x13_y3.png</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.0048</v>
+        <v>0.0276</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_4.png</t>
+          <t>P_006_quad_crp_x13_y4.png</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.1156</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_5.png</t>
+          <t>P_006_quad_crp_x13_y5.png</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.0328</v>
+        <v>0.0476</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_6.png</t>
+          <t>P_006_quad_crp_x13_y6.png</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.1732</v>
+        <v>0.2168</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_7.png</t>
+          <t>P_006_quad_crp_x13_y7.png</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.0544</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_8.png</t>
+          <t>P_006_quad_crp_x13_y8.png</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.028</v>
+        <v>0.0436</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_9.png</t>
+          <t>P_006_quad_crp_x13_y9.png</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.0152</v>
+        <v>0.0324</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_10.png</t>
+          <t>P_006_quad_crp_x13_y10.png</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.0568</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_11.png</t>
+          <t>P_006_quad_crp_x13_y11.png</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>0.0776</v>
+        <v>0.0984</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_12.png</t>
+          <t>P_006_quad_crp_x13_y12.png</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>0.1416</v>
+        <v>0.1716</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_13.png</t>
+          <t>P_006_quad_crp_x13_y13.png</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.0436</v>
+        <v>0.2076</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>P_006_quad_crp_x_13_y_14.png</t>
+          <t>P_006_quad_crp_x13_y14.png</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.3912</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Einfügen der Drehen-Funktion der großen Bilder
</commit_message>
<xml_diff>
--- a/Bildervorbearbeitung/Bilder/xlsx/Porositaet_P_006_quad.xlsx
+++ b/Bildervorbearbeitung/Bilder/xlsx/Porositaet_P_006_quad.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1236</v>
+        <v>0.09039999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1048</v>
+        <v>0.0804</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0344</v>
+        <v>0.0216</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1728</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1852</v>
+        <v>0.1436</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1516</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0396</v>
+        <v>0.0256</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0824</v>
+        <v>0.0532</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1172</v>
+        <v>0.08400000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.06520000000000001</v>
+        <v>0.04960000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1048</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4</v>
+        <v>0.326</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.09279999999999999</v>
+        <v>0.0588</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.034</v>
+        <v>0.0212</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.236</v>
+        <v>0.1976</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07479999999999999</v>
+        <v>0.0484</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1596</v>
+        <v>0.1124</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.1824</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.2628</v>
+        <v>0.1892</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.022</v>
+        <v>0.0132</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.2512</v>
+        <v>0.2128</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.11</v>
+        <v>0.0672</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1008</v>
+        <v>0.06319999999999999</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1576</v>
+        <v>0.1264</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.06560000000000001</v>
+        <v>0.0328</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.3128</v>
+        <v>0.2528</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.2016</v>
+        <v>0.1692</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.0448</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.0464</v>
+        <v>0.0212</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.0332</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.0248</v>
+        <v>0.008399999999999999</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1808</v>
+        <v>0.1516</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1888</v>
+        <v>0.1404</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.0588</v>
+        <v>0.0412</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.2284</v>
+        <v>0.198</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.2052</v>
+        <v>0.1652</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.3024</v>
+        <v>0.1932</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.0444</v>
+        <v>0.0252</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.1624</v>
+        <v>0.106</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.1892</v>
+        <v>0.1276</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.08639999999999999</v>
+        <v>0.0588</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.0292</v>
+        <v>0.0136</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.24</v>
+        <v>0.2084</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.0404</v>
+        <v>0.0224</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.0264</v>
+        <v>0.0152</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.0296</v>
+        <v>0.0192</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.0832</v>
+        <v>0.06279999999999999</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.1036</v>
+        <v>0.0832</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.0456</v>
+        <v>0.0336</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.0168</v>
+        <v>0.008399999999999999</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.1324</v>
+        <v>0.0956</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.2896</v>
+        <v>0.256</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.0592</v>
+        <v>0.0344</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.05159999999999999</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.0712</v>
+        <v>0.0488</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.1688</v>
+        <v>0.1356</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.05959999999999999</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.0504</v>
+        <v>0.0372</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0508</v>
+        <v>0.0304</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.022</v>
+        <v>0.0112</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.066</v>
+        <v>0.0492</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.1092</v>
+        <v>0.07919999999999999</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.0492</v>
+        <v>0.0316</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.0824</v>
+        <v>0.0548</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.07240000000000001</v>
+        <v>0.0572</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.1316</v>
+        <v>0.1068</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.8736</v>
+        <v>0.7396</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.0408</v>
+        <v>0.0196</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.1216</v>
+        <v>0.08800000000000001</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.044</v>
+        <v>0.0144</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.08760000000000001</v>
+        <v>0.0616</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.0956</v>
+        <v>0.06999999999999999</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.09719999999999999</v>
+        <v>0.0832</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.0212</v>
+        <v>0.0092</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.0148</v>
+        <v>0.0068</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.066</v>
+        <v>0.04960000000000001</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.0484</v>
+        <v>0.0316</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>1.0172</v>
+        <v>0.9608</v>
       </c>
     </row>
     <row r="80">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.06759999999999999</v>
+        <v>0.0412</v>
       </c>
     </row>
     <row r="81">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.1744</v>
+        <v>0.1332</v>
       </c>
     </row>
     <row r="82">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.22</v>
+        <v>0.1536</v>
       </c>
     </row>
     <row r="83">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.098</v>
+        <v>0.0716</v>
       </c>
     </row>
     <row r="84">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.0648</v>
+        <v>0.0512</v>
       </c>
     </row>
     <row r="85">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.0552</v>
+        <v>0.0308</v>
       </c>
     </row>
     <row r="86">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.0912</v>
+        <v>0.0668</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.228</v>
+        <v>0.194</v>
       </c>
     </row>
     <row r="88">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.146</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="89">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.0392</v>
+        <v>0.0196</v>
       </c>
     </row>
     <row r="90">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.03759999999999999</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="91">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.1112</v>
+        <v>0.08639999999999999</v>
       </c>
     </row>
     <row r="92">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.266</v>
+        <v>0.2164</v>
       </c>
     </row>
     <row r="93">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.014</v>
+        <v>0.0052</v>
       </c>
     </row>
     <row r="94">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.0956</v>
+        <v>0.0616</v>
       </c>
     </row>
     <row r="95">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.1776</v>
+        <v>0.136</v>
       </c>
     </row>
     <row r="96">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.2856</v>
+        <v>0.2552</v>
       </c>
     </row>
     <row r="97">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.06080000000000001</v>
+        <v>0.03759999999999999</v>
       </c>
     </row>
     <row r="98">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.0232</v>
+        <v>0.0092</v>
       </c>
     </row>
     <row r="99">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.0444</v>
+        <v>0.0148</v>
       </c>
     </row>
     <row r="100">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.1468</v>
+        <v>0.1188</v>
       </c>
     </row>
     <row r="101">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.08639999999999999</v>
+        <v>0.0612</v>
       </c>
     </row>
     <row r="102">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.0296</v>
+        <v>0.0144</v>
       </c>
     </row>
     <row r="103">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.0176</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="104">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.1792</v>
+        <v>0.1532</v>
       </c>
     </row>
     <row r="105">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.2928</v>
+        <v>0.2632</v>
       </c>
     </row>
     <row r="106">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.0296</v>
+        <v>0.0164</v>
       </c>
     </row>
     <row r="107">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.066</v>
+        <v>0.0428</v>
       </c>
     </row>
     <row r="108">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.1864</v>
+        <v>0.1444</v>
       </c>
     </row>
     <row r="109">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.2</v>
+        <v>0.1652</v>
       </c>
     </row>
     <row r="110">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.1124</v>
+        <v>0.0716</v>
       </c>
     </row>
     <row r="111">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.1328</v>
+        <v>0.1032</v>
       </c>
     </row>
     <row r="112">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.3588</v>
+        <v>0.2948</v>
       </c>
     </row>
     <row r="113">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.1632</v>
+        <v>0.1232</v>
       </c>
     </row>
     <row r="114">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.0188</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="115">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.014</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="116">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.0304</v>
+        <v>0.0172</v>
       </c>
     </row>
     <row r="117">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.0704</v>
+        <v>0.0448</v>
       </c>
     </row>
     <row r="118">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.1832</v>
+        <v>0.1528</v>
       </c>
     </row>
     <row r="119">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.06999999999999999</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="120">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.1184</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="121">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.0552</v>
+        <v>0.0372</v>
       </c>
     </row>
     <row r="122">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.1692</v>
+        <v>0.1324</v>
       </c>
     </row>
     <row r="123">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.2636</v>
+        <v>0.2296</v>
       </c>
     </row>
     <row r="124">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>0.4072</v>
+        <v>0.3144</v>
       </c>
     </row>
     <row r="125">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>0.0716</v>
+        <v>0.048</v>
       </c>
     </row>
     <row r="126">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>0.1728</v>
+        <v>0.1396</v>
       </c>
     </row>
     <row r="127">
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0.1332</v>
+        <v>0.1024</v>
       </c>
     </row>
     <row r="128">
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>0.036</v>
+        <v>0.0104</v>
       </c>
     </row>
     <row r="129">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.028</v>
+        <v>0.0148</v>
       </c>
     </row>
     <row r="130">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.1156</v>
+        <v>0.0872</v>
       </c>
     </row>
     <row r="131">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.0164</v>
+        <v>0.006399999999999999</v>
       </c>
     </row>
     <row r="132">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="133">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.0776</v>
+        <v>0.0616</v>
       </c>
     </row>
     <row r="134">
@@ -1772,7 +1772,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.0944</v>
+        <v>0.0772</v>
       </c>
     </row>
     <row r="135">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.098</v>
+        <v>0.0696</v>
       </c>
     </row>
     <row r="136">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.0448</v>
+        <v>0.0224</v>
       </c>
     </row>
     <row r="137">
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.1312</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="138">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.0456</v>
+        <v>0.0204</v>
       </c>
     </row>
     <row r="139">
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.128</v>
+        <v>0.0776</v>
       </c>
     </row>
     <row r="140">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.1612</v>
+        <v>0.1104</v>
       </c>
     </row>
     <row r="141">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.2636</v>
+        <v>0.1896</v>
       </c>
     </row>
     <row r="142">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.0872</v>
+        <v>0.0504</v>
       </c>
     </row>
     <row r="143">
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.0216</v>
+        <v>0.0108</v>
       </c>
     </row>
     <row r="144">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.1752</v>
+        <v>0.1328</v>
       </c>
     </row>
     <row r="145">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.0648</v>
+        <v>0.0384</v>
       </c>
     </row>
     <row r="146">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.1096</v>
+        <v>0.0868</v>
       </c>
     </row>
     <row r="147">
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.0256</v>
+        <v>0.0092</v>
       </c>
     </row>
     <row r="148">
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.0152</v>
+        <v>0.0052</v>
       </c>
     </row>
     <row r="149">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.0384</v>
+        <v>0.0256</v>
       </c>
     </row>
     <row r="150">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.0464</v>
+        <v>0.0176</v>
       </c>
     </row>
     <row r="151">
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.098</v>
+        <v>0.07479999999999999</v>
       </c>
     </row>
     <row r="152">
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.0916</v>
+        <v>0.0664</v>
       </c>
     </row>
     <row r="153">
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>0.5868</v>
+        <v>0.5232</v>
       </c>
     </row>
     <row r="154">
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.208</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="155">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0.04960000000000001</v>
+        <v>0.0232</v>
       </c>
     </row>
     <row r="156">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.0556</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="157">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.118</v>
+        <v>0.0848</v>
       </c>
     </row>
     <row r="158">
@@ -2012,7 +2012,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.1584</v>
+        <v>0.124</v>
       </c>
     </row>
     <row r="159">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.2072</v>
+        <v>0.1812</v>
       </c>
     </row>
     <row r="160">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.1104</v>
+        <v>0.08800000000000001</v>
       </c>
     </row>
     <row r="161">
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.0292</v>
+        <v>0.0152</v>
       </c>
     </row>
     <row r="162">
@@ -2052,7 +2052,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.0544</v>
+        <v>0.0348</v>
       </c>
     </row>
     <row r="163">
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.066</v>
+        <v>0.0268</v>
       </c>
     </row>
     <row r="164">
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.1652</v>
+        <v>0.1228</v>
       </c>
     </row>
     <row r="165">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.1008</v>
+        <v>0.0692</v>
       </c>
     </row>
     <row r="166">
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.0832</v>
+        <v>0.0544</v>
       </c>
     </row>
     <row r="167">
@@ -2102,7 +2102,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.0452</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="168">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.296</v>
+        <v>0.2264</v>
       </c>
     </row>
     <row r="169">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.0388</v>
+        <v>0.0196</v>
       </c>
     </row>
     <row r="170">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.1692</v>
+        <v>0.1188</v>
       </c>
     </row>
     <row r="171">
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.0624</v>
+        <v>0.0216</v>
       </c>
     </row>
     <row r="172">
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.0276</v>
+        <v>0.0048</v>
       </c>
     </row>
     <row r="173">
@@ -2162,7 +2162,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.1156</v>
+        <v>0.08599999999999999</v>
       </c>
     </row>
     <row r="174">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.0476</v>
+        <v>0.0328</v>
       </c>
     </row>
     <row r="175">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.2168</v>
+        <v>0.1732</v>
       </c>
     </row>
     <row r="176">
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.082</v>
+        <v>0.0544</v>
       </c>
     </row>
     <row r="177">
@@ -2202,7 +2202,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.0436</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="178">
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.0324</v>
+        <v>0.0152</v>
       </c>
     </row>
     <row r="179">
@@ -2222,7 +2222,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.082</v>
+        <v>0.0568</v>
       </c>
     </row>
     <row r="180">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>0.0984</v>
+        <v>0.0776</v>
       </c>
     </row>
     <row r="181">
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>0.1716</v>
+        <v>0.1416</v>
       </c>
     </row>
     <row r="182">
@@ -2252,7 +2252,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.2076</v>
+        <v>0.0436</v>
       </c>
     </row>
     <row r="183">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.75</v>
+        <v>0.3912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>